<commit_message>
Add wheels and frames selection
</commit_message>
<xml_diff>
--- a/rides.xlsx
+++ b/rides.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="109">
   <si>
     <t xml:space="preserve">dtime</t>
   </si>
@@ -341,6 +341,12 @@
   </si>
   <si>
     <t xml:space="preserve">1:21:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-06-19 17:34:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy ENVE SES 3.4 wheel</t>
   </si>
 </sst>
 </file>
@@ -466,13 +472,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.24"/>
@@ -2375,6 +2381,24 @@
         <v>63</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>-191700</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <f aca="false">M28+L29</f>
+        <v>301732</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>